<commit_message>
- changed after used ChatGPT. - changes before adding dateFormatting due to the problem with the month february
</commit_message>
<xml_diff>
--- a/src/main/resources/2022.01.xlsx
+++ b/src/main/resources/2022.01.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cvbn\IdeaProjects\TaxiRechnungen\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekoca/Desktop/Persönlich/TaxiRechnungen/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F610EAA4-A9A2-4FCC-8F33-04FB3AE2E582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCF4DFA-09A7-944D-BD61-15F250258446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E29335DA-9D6A-4D4F-89C3-F989C8FC26CC}"/>
+    <workbookView xWindow="3300" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{E29335DA-9D6A-4D4F-89C3-F989C8FC26CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,8 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Taxi &amp; Transportkurier Ahmet Koca</t>
   </si>
   <si>
-    <t>Neuweilerstrasse 88</t>
-  </si>
-  <si>
-    <t>4054 Basel</t>
-  </si>
-  <si>
     <t>Telefon: 079 644 08 40</t>
   </si>
   <si>
@@ -85,9 +83,6 @@
     <t>Rückfahrt: Von Dychrain nach Hause, 16:30 Uhr</t>
   </si>
   <si>
-    <t>Summe Total:</t>
-  </si>
-  <si>
     <t>Hinfahrt: Von Zuhause nach Dychrain, 8:30 Uhr</t>
   </si>
   <si>
@@ -98,6 +93,18 @@
   </si>
   <si>
     <t>Abrechnungsperiode: 01.01.2022 – 31.01.2022</t>
+  </si>
+  <si>
+    <t>MwSt Nr: CHE-108.242.406</t>
+  </si>
+  <si>
+    <t>Summe Total inkl. 7.7% MwSt:</t>
+  </si>
+  <si>
+    <t>Im Westfeld 17</t>
+  </si>
+  <si>
+    <t>4055 Basel</t>
   </si>
 </sst>
 </file>
@@ -220,7 +227,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -236,7 +243,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -534,53 +541,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BC3C87-E7E4-4331-8117-DBD5106A4834}">
   <dimension ref="A2:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H2" s="15"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
       <c r="I3" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="I4" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I6" s="8"/>
       <c r="K6" s="3"/>
       <c r="L6" s="9"/>
@@ -588,9 +595,9 @@
       <c r="N6" s="8"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H7" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I7" s="8"/>
       <c r="K7" s="3"/>
@@ -599,9 +606,9 @@
       <c r="N7" s="8"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H8" s="14">
         <v>44592</v>
@@ -613,7 +620,7 @@
       <c r="N8" s="8"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I9" s="8"/>
       <c r="K9" s="3"/>
       <c r="L9" s="9"/>
@@ -621,7 +628,7 @@
       <c r="N9" s="8"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I10" s="8"/>
       <c r="K10" s="3"/>
       <c r="L10" s="9"/>
@@ -629,7 +636,7 @@
       <c r="N10" s="8"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I11" s="8"/>
       <c r="K11" s="3"/>
       <c r="L11" s="9"/>
@@ -637,7 +644,7 @@
       <c r="N11" s="8"/>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I12" s="8"/>
       <c r="K12" s="3"/>
       <c r="L12" s="9"/>
@@ -645,7 +652,7 @@
       <c r="N12" s="8"/>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I13" s="8"/>
       <c r="K13" s="3"/>
       <c r="L13" s="9"/>
@@ -653,12 +660,12 @@
       <c r="N13" s="8"/>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="I14" s="8"/>
       <c r="K14" s="3"/>
@@ -667,12 +674,12 @@
       <c r="N14" s="8"/>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="I15" s="8"/>
       <c r="K15" s="3"/>
@@ -681,12 +688,12 @@
       <c r="N15" s="8"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I16" s="8"/>
       <c r="K16" s="3"/>
@@ -695,9 +702,9 @@
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I17" s="8"/>
       <c r="K17" s="3"/>
@@ -706,7 +713,7 @@
       <c r="N17" s="8"/>
       <c r="O17" s="9"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I18" s="8"/>
       <c r="K18" s="3"/>
       <c r="L18" s="9"/>
@@ -714,7 +721,7 @@
       <c r="N18" s="8"/>
       <c r="O18" s="9"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I19" s="8"/>
       <c r="K19" s="3"/>
       <c r="L19" s="9"/>
@@ -722,7 +729,7 @@
       <c r="N19" s="8"/>
       <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I20" s="8"/>
       <c r="K20" s="3"/>
       <c r="L20" s="9"/>
@@ -730,7 +737,7 @@
       <c r="N20" s="8"/>
       <c r="O20" s="9"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I21" s="8"/>
       <c r="K21" s="3"/>
       <c r="L21" s="9"/>
@@ -738,9 +745,9 @@
       <c r="N21" s="8"/>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C22" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D22" s="12">
         <f>O42</f>
@@ -753,7 +760,7 @@
       <c r="N22" s="8"/>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I23" s="8"/>
       <c r="K23" s="3"/>
       <c r="L23" s="9"/>
@@ -761,7 +768,7 @@
       <c r="N23" s="8"/>
       <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I24" s="8"/>
       <c r="K24" s="3"/>
       <c r="L24" s="9"/>
@@ -769,7 +776,7 @@
       <c r="N24" s="8"/>
       <c r="O24" s="9"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I25" s="8"/>
       <c r="K25" s="3"/>
       <c r="L25" s="9"/>
@@ -777,7 +784,7 @@
       <c r="N25" s="8"/>
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I26" s="8"/>
       <c r="K26" s="3"/>
       <c r="L26" s="9"/>
@@ -785,7 +792,7 @@
       <c r="N26" s="8"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I27" s="8"/>
       <c r="K27" s="3"/>
       <c r="L27" s="9"/>
@@ -793,7 +800,7 @@
       <c r="N27" s="8"/>
       <c r="O27" s="9"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I28" s="8"/>
       <c r="K28" s="3"/>
       <c r="L28" s="9"/>
@@ -801,9 +808,9 @@
       <c r="N28" s="8"/>
       <c r="O28" s="9"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I29" s="8"/>
       <c r="K29" s="3"/>
@@ -812,7 +819,7 @@
       <c r="N29" s="8"/>
       <c r="O29" s="9"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I30" s="8"/>
       <c r="K30" s="3"/>
       <c r="L30" s="9"/>
@@ -820,7 +827,7 @@
       <c r="N30" s="8"/>
       <c r="O30" s="9"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -831,9 +838,9 @@
       <c r="N31" s="8"/>
       <c r="O31" s="9"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I32" s="8"/>
       <c r="K32" s="3"/>
@@ -842,9 +849,9 @@
       <c r="N32" s="8"/>
       <c r="O32" s="9"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I33" s="8"/>
       <c r="K33" s="3"/>
@@ -853,9 +860,9 @@
       <c r="N33" s="8"/>
       <c r="O33" s="9"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I34" s="8"/>
       <c r="K34" s="3"/>
@@ -864,7 +871,10 @@
       <c r="N34" s="8"/>
       <c r="O34" s="9"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="I35" s="8"/>
       <c r="K35" s="3"/>
       <c r="L35" s="9"/>
@@ -872,7 +882,7 @@
       <c r="N35" s="8"/>
       <c r="O35" s="9"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I36" s="8"/>
       <c r="K36" s="3"/>
       <c r="L36" s="9"/>
@@ -880,7 +890,7 @@
       <c r="N36" s="8"/>
       <c r="O36" s="9"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I37" s="8"/>
       <c r="K37" s="3"/>
       <c r="L37" s="9"/>
@@ -888,7 +898,7 @@
       <c r="N37" s="8"/>
       <c r="O37" s="9"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I38" s="8"/>
       <c r="K38" s="3"/>
       <c r="L38" s="9"/>
@@ -896,7 +906,7 @@
       <c r="N38" s="8"/>
       <c r="O38" s="9"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I39" s="8"/>
       <c r="K39" s="3"/>
       <c r="L39" s="9"/>
@@ -904,9 +914,9 @@
       <c r="N39" s="8"/>
       <c r="O39" s="9"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I40" s="8"/>
       <c r="K40" s="3"/>
@@ -915,15 +925,15 @@
       <c r="N40" s="8"/>
       <c r="O40" s="9"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M42" s="7" t="s">
-        <v>17</v>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L42" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="O42" s="11"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="D44" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +941,7 @@
     <mergeCell ref="G2:H3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.51181102362204722" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding rounding into the total price
</commit_message>
<xml_diff>
--- a/src/main/resources/2022.01.xlsx
+++ b/src/main/resources/2022.01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekoca/Desktop/Persönlich/TaxiRechnungen/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCF4DFA-09A7-944D-BD61-15F250258446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104CAFED-53E2-C04F-BB4E-1FECDE33E377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{E29335DA-9D6A-4D4F-89C3-F989C8FC26CC}"/>
   </bookViews>
@@ -98,13 +98,13 @@
     <t>MwSt Nr: CHE-108.242.406</t>
   </si>
   <si>
-    <t>Summe Total inkl. 7.7% MwSt:</t>
-  </si>
-  <si>
     <t>Im Westfeld 17</t>
   </si>
   <si>
     <t>4055 Basel</t>
+  </si>
+  <si>
+    <t>Summe Total inkl. 8.1% MwSt:</t>
   </si>
 </sst>
 </file>
@@ -243,9 +243,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -283,7 +283,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -389,7 +389,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -531,7 +531,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BC3C87-E7E4-4331-8117-DBD5106A4834}">
   <dimension ref="A2:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -566,7 +566,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -690,7 +690,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>18</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I17" s="8"/>
       <c r="K17" s="3"/>
@@ -927,7 +927,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L42" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O42" s="11"/>
     </row>

</xml_diff>